<commit_message>
SMI cumulative distribution function
</commit_message>
<xml_diff>
--- a/soilwater_holding_characteristics.xlsx
+++ b/soilwater_holding_characteristics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\VUB\_main_research\mHM\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121A95B2-77FD-45A8-98E4-EA416AD25CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581FEF88-3D55-4852-A2B4-E9596A1A3FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47040" yWindow="3090" windowWidth="24825" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30750" yWindow="1950" windowWidth="24825" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -627,11 +627,11 @@
         <v>1.4304019345272008</v>
       </c>
       <c r="N3" s="1">
-        <f>$B$18*(I3)/100</f>
+        <f t="shared" ref="N3:N13" si="3">$B$18*(I3)/100</f>
         <v>20.785573525222517</v>
       </c>
       <c r="O3" s="1">
-        <f t="shared" ref="O3:O13" si="3">$B$18*(J3)/100</f>
+        <f t="shared" ref="O3:O13" si="4">$B$18*(J3)/100</f>
         <v>122.77991552522256</v>
       </c>
     </row>
@@ -676,11 +676,11 @@
         <v>1.4577791733376451</v>
       </c>
       <c r="N4" s="1">
-        <f>$B$18*(I4)/100</f>
+        <f t="shared" si="3"/>
         <v>29.519193471209984</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>110.73730547120998</v>
       </c>
     </row>
@@ -725,11 +725,11 @@
         <v>1.4323826509068802</v>
       </c>
       <c r="N5" s="1">
-        <f>$B$18*(I5)/100</f>
+        <f t="shared" si="3"/>
         <v>42.775969482239972</v>
       </c>
       <c r="O5" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>96.736393482239976</v>
       </c>
     </row>
@@ -774,11 +774,11 @@
         <v>1.3813789264670113</v>
       </c>
       <c r="N6" s="1">
-        <f>$B$18*(I6)/100</f>
+        <f t="shared" si="3"/>
         <v>58.595956022602508</v>
       </c>
       <c r="O6" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>110.65855002260248</v>
       </c>
     </row>
@@ -823,11 +823,11 @@
         <v>1.3805687930378112</v>
       </c>
       <c r="N7" s="1">
-        <f>$B$18*(I7)/100</f>
+        <f t="shared" si="3"/>
         <v>74.135449241002505</v>
       </c>
       <c r="O7" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>126.48226324100247</v>
       </c>
     </row>
@@ -872,11 +872,11 @@
         <v>1.4995535125215311</v>
       </c>
       <c r="N8" s="1">
-        <f>$B$18*(I8)/100</f>
+        <f t="shared" si="3"/>
         <v>30.393164997562486</v>
       </c>
       <c r="O8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>80.518874997562506</v>
       </c>
     </row>
@@ -921,11 +921,11 @@
         <v>1.3853121630553114</v>
       </c>
       <c r="N9" s="1">
-        <f>$B$18*(I9)/100</f>
+        <f t="shared" si="3"/>
         <v>41.97174395600252</v>
       </c>
       <c r="O9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>77.774577956002489</v>
       </c>
     </row>
@@ -970,11 +970,11 @@
         <v>1.2952670987944512</v>
       </c>
       <c r="N10" s="1">
-        <f>$B$18*(I10)/100</f>
+        <f t="shared" si="3"/>
         <v>49.994220815722485</v>
       </c>
       <c r="O10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>88.809678815722492</v>
       </c>
     </row>
@@ -1019,11 +1019,11 @@
         <v>1.2627770209239111</v>
       </c>
       <c r="N11" s="1">
-        <f>$B$18*(I11)/100</f>
+        <f t="shared" si="3"/>
         <v>42.406334838802508</v>
       </c>
       <c r="O11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>76.711340838802514</v>
       </c>
     </row>
@@ -1068,11 +1068,11 @@
         <v>1.4739567575004997</v>
       </c>
       <c r="N12" s="1">
-        <f>$B$18*(I12)/100</f>
+        <f t="shared" si="3"/>
         <v>33.742230849000009</v>
       </c>
       <c r="O12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>58.544670849000028</v>
       </c>
     </row>
@@ -1117,11 +1117,11 @@
         <v>1.329148230003125</v>
       </c>
       <c r="N13" s="1">
-        <f>$B$18*(I13)/100</f>
+        <f t="shared" si="3"/>
         <v>36.81393905625</v>
       </c>
       <c r="O13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>60.155139056250022</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ET validation plots
</commit_message>
<xml_diff>
--- a/soilwater_holding_characteristics.xlsx
+++ b/soilwater_holding_characteristics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\VUB\_main_research\mHM\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{581FEF88-3D55-4852-A2B4-E9596A1A3FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F7259C-1D5E-47B4-A409-37A1DE6DB472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30750" yWindow="1950" windowWidth="24825" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24825" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Compute Soil Moisture Anomaly according to European Drought Observatory
</commit_message>
<xml_diff>
--- a/soilwater_holding_characteristics.xlsx
+++ b/soilwater_holding_characteristics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\VUB\_main_research\mHM\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F7259C-1D5E-47B4-A409-37A1DE6DB472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EF7145-F496-49E5-B433-4EF73D3FD356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24825" windowHeight="17385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="165" windowWidth="29010" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Texture</t>
   </si>
@@ -117,6 +117,24 @@
   </si>
   <si>
     <t>TWC_mm</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>ssat</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>I</t>
   </si>
 </sst>
 </file>
@@ -471,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1130,9 +1148,54 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="B18" s="1">
         <v>300</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G20" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F24" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G24" s="1">
+        <f>EXP(G21*LN(G19/G20))</f>
+        <v>0.81649658092772603</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G25" s="1">
+        <f>(G19/G20)^G21</f>
+        <v>0.81649658092772603</v>
       </c>
     </row>
   </sheetData>

</xml_diff>